<commit_message>
EPBDS-9039 Incorrect Cast happens if input value and condition have different types.
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9039_IndexAndNoIndexDTWithDifferentTypesV1.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9039_IndexAndNoIndexDTWithDifferentTypesV1.xlsx
@@ -5,22 +5,22 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkama\.openl\user-workspace\DEFAULT\EPBDS-9039_IndexAndNoIndexDTWithDifferentTypes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE2FA08-58CD-4B71-B026-3953F7B32428}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C26029-3585-44F9-920B-5FBAF3EE3003}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5693" yWindow="2318" windowWidth="21600" windowHeight="11535" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5693" yWindow="2318" windowWidth="21600" windowHeight="11535" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Range" sheetId="2" r:id="rId1"/>
-    <sheet name="RangeContains" sheetId="5" r:id="rId2"/>
-    <sheet name="Range_DependentParams" sheetId="4" r:id="rId3"/>
-    <sheet name="Range_2_Columns" sheetId="7" r:id="rId4"/>
-    <sheet name="Range_2_Column_Expression" sheetId="8" r:id="rId5"/>
-    <sheet name="Equals" sheetId="3" r:id="rId6"/>
-    <sheet name="Equals_Expression" sheetId="6" r:id="rId7"/>
-    <sheet name="Contains" sheetId="9" r:id="rId8"/>
+    <sheet name="Range_DependentParams" sheetId="4" r:id="rId2"/>
+    <sheet name="Range_2_Columns" sheetId="7" r:id="rId3"/>
+    <sheet name="Range_2_Column_Expression" sheetId="8" r:id="rId4"/>
+    <sheet name="Equals" sheetId="3" r:id="rId5"/>
+    <sheet name="Equals_Expression" sheetId="6" r:id="rId6"/>
+    <sheet name="Contains" sheetId="9" r:id="rId7"/>
+    <sheet name="Contains_Expression" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="114">
   <si>
     <t>C1</t>
   </si>
@@ -153,156 +153,6 @@
     <t>x.contains(param)</t>
   </si>
   <si>
-    <t>Spreadsheet SpreadsheetResult RangeContains()</t>
-  </si>
-  <si>
-    <t>Step</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>byte</t>
-  </si>
-  <si>
-    <t>short</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>long</t>
-  </si>
-  <si>
-    <t>float</t>
-  </si>
-  <si>
-    <t>double</t>
-  </si>
-  <si>
-    <t>Byte</t>
-  </si>
-  <si>
-    <t>Short</t>
-  </si>
-  <si>
-    <t>Long</t>
-  </si>
-  <si>
-    <t>Float</t>
-  </si>
-  <si>
-    <t>BigInteger</t>
-  </si>
-  <si>
-    <t>BigDecimal</t>
-  </si>
-  <si>
-    <t>ByteValue</t>
-  </si>
-  <si>
-    <t>ShortValue</t>
-  </si>
-  <si>
-    <t>IntValue</t>
-  </si>
-  <si>
-    <t>LongValue</t>
-  </si>
-  <si>
-    <t>FloatValue</t>
-  </si>
-  <si>
-    <t>DoubleValue</t>
-  </si>
-  <si>
-    <t>BigIntegerValue</t>
-  </si>
-  <si>
-    <t>BigDecimalValue</t>
-  </si>
-  <si>
-    <t>= new IntRange("-1; 1")</t>
-  </si>
-  <si>
-    <t>ContainsInIntRange</t>
-  </si>
-  <si>
-    <t>= $Value$IntRange.contains($Value)</t>
-  </si>
-  <si>
-    <t>= (byte) 0</t>
-  </si>
-  <si>
-    <t>= (short) 0</t>
-  </si>
-  <si>
-    <t>= (int) 0</t>
-  </si>
-  <si>
-    <t>= (long) 0</t>
-  </si>
-  <si>
-    <t>= (float) 0</t>
-  </si>
-  <si>
-    <t>= (double) 0</t>
-  </si>
-  <si>
-    <t>= (Byte) 0</t>
-  </si>
-  <si>
-    <t>= (Short) 0</t>
-  </si>
-  <si>
-    <t>= (Integer) 0</t>
-  </si>
-  <si>
-    <t>= (Long) 0</t>
-  </si>
-  <si>
-    <t>= (Float) 0</t>
-  </si>
-  <si>
-    <t>= (Double) 0</t>
-  </si>
-  <si>
-    <t>= (BigInteger) 0</t>
-  </si>
-  <si>
-    <t>= (BigDecimal) 0</t>
-  </si>
-  <si>
-    <t>= (ByteValue) 0</t>
-  </si>
-  <si>
-    <t>= (ShortValue) 0</t>
-  </si>
-  <si>
-    <t>= (IntValue) 0</t>
-  </si>
-  <si>
-    <t>= (LongValue) 0</t>
-  </si>
-  <si>
-    <t>= (FloatValue) 0</t>
-  </si>
-  <si>
-    <t>= (DoubleValue) 0</t>
-  </si>
-  <si>
-    <t>= (BigIntegerValue) 0</t>
-  </si>
-  <si>
-    <t>= (BigDecimalValue) 0</t>
-  </si>
-  <si>
-    <t>= $Value$DoubleRange.contains($Value)</t>
-  </si>
-  <si>
-    <t>= new DoubleRange("-1; 1")</t>
-  </si>
-  <si>
     <t>((DoubleRange)x).contains(param)</t>
   </si>
   <si>
@@ -493,6 +343,39 @@
   </si>
   <si>
     <t>Test  indexContainsDouble_ParamInteger indexContainsDouble_ParamIntegerTest</t>
+  </si>
+  <si>
+    <t>Rules Integer indexContainsInteger_Expression_ParamDouble(Double param)</t>
+  </si>
+  <si>
+    <t>Test  indexContainsInteger_Expression_ParamDouble indexContainsInteger_Expression_ParamDoubleTest</t>
+  </si>
+  <si>
+    <t>Rules Integer indexContainsDouble_Expression_ParamInteger(Integer param)</t>
+  </si>
+  <si>
+    <t>Test  indexContainsDouble_Expression_ParamInteger indexContainsDouble_Expression_ParamIntegerTest</t>
+  </si>
+  <si>
+    <t>Rules Integer noIndexContainsInteger_Expression_ParamDouble(Double param)</t>
+  </si>
+  <si>
+    <t>Test  noIndexContainsInteger_Expression_ParamDouble noIndexContainsInteger_Expression_ParamDoubleTest</t>
+  </si>
+  <si>
+    <t>Rules Integer noIndexContainsDouble_Expression_ParamInteger(Integer param)</t>
+  </si>
+  <si>
+    <t>Test  noIndexContainsDouble_Expression_ParamInteger noIndexContainsDouble_Expression_ParamIntegerTest</t>
+  </si>
+  <si>
+    <t>contains(x, param)</t>
+  </si>
+  <si>
+    <t>Integer[] x</t>
+  </si>
+  <si>
+    <t>Double[] x</t>
   </si>
 </sst>
 </file>
@@ -1451,353 +1334,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3FA0FE-50FB-4DE6-8A36-72A3D50C02EA}">
-  <dimension ref="B4:E29"/>
-  <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="3" max="3" width="20.06640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="30.46484375" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B14" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B18" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B20" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B22" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B23" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B24" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B25" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B26" t="s">
-        <v>58</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B27" t="s">
-        <v>59</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B28" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.45">
-      <c r="B29" t="s">
-        <v>61</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA0AAF78-1E59-425E-A306-262A8A76F550}">
   <dimension ref="B3:C69"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
@@ -1819,7 +1359,7 @@
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B5" s="3" t="s">
-        <v>89</v>
+        <v>39</v>
       </c>
       <c r="C5" s="3"/>
     </row>
@@ -1931,7 +1471,7 @@
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B22" s="3" t="s">
-        <v>89</v>
+        <v>39</v>
       </c>
       <c r="C22" s="3"/>
     </row>
@@ -2248,7 +1788,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EBBA327-A503-4137-A681-2390B6DD3420}">
   <dimension ref="B3:D70"/>
   <sheetViews>
@@ -2266,7 +1806,7 @@
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B3" s="6" t="s">
-        <v>108</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.45">
@@ -2294,10 +1834,10 @@
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B7" s="7" t="s">
-        <v>116</v>
+        <v>66</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>117</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.45">
@@ -2329,7 +1869,7 @@
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B12" s="6" t="s">
-        <v>109</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.45">
@@ -2374,7 +1914,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B20" s="6" t="s">
-        <v>110</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.45">
@@ -2402,10 +1942,10 @@
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B24" s="7" t="s">
-        <v>116</v>
+        <v>66</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>117</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.45">
@@ -2421,10 +1961,10 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B26" s="8" t="s">
-        <v>118</v>
+        <v>68</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>119</v>
+        <v>69</v>
       </c>
       <c r="D26" s="6">
         <v>2</v>
@@ -2437,7 +1977,7 @@
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B29" s="6" t="s">
-        <v>111</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.45">
@@ -2474,7 +2014,7 @@
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B36" s="6" t="s">
-        <v>112</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.45">
@@ -2502,10 +2042,10 @@
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B40" s="7" t="s">
-        <v>116</v>
+        <v>66</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>117</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.45">
@@ -2548,7 +2088,7 @@
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B47" s="6" t="s">
-        <v>113</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.45">
@@ -2593,7 +2133,7 @@
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B54" s="6" t="s">
-        <v>114</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.45">
@@ -2621,10 +2161,10 @@
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B58" s="7" t="s">
-        <v>116</v>
+        <v>66</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>117</v>
+        <v>67</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.45">
@@ -2654,7 +2194,7 @@
         <v>23</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="D61" s="6">
         <v>3</v>
@@ -2667,7 +2207,7 @@
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B65" s="6" t="s">
-        <v>115</v>
+        <v>65</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.45">
@@ -2725,7 +2265,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAEE3FEA-B42F-4DA8-AFDC-3595C7CB86E9}">
   <dimension ref="B3:D70"/>
   <sheetViews>
@@ -2743,7 +2283,7 @@
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B3" s="6" t="s">
-        <v>121</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.45">
@@ -2757,24 +2297,24 @@
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B5" s="10" t="s">
-        <v>129</v>
+        <v>79</v>
       </c>
       <c r="C5" s="10"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B6" s="7" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B7" s="7" t="s">
-        <v>116</v>
+        <v>66</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>117</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.45">
@@ -2806,7 +2346,7 @@
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B12" s="6" t="s">
-        <v>122</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.45">
@@ -2851,7 +2391,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B20" s="6" t="s">
-        <v>123</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.45">
@@ -2865,24 +2405,24 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B22" s="10" t="s">
-        <v>134</v>
+        <v>84</v>
       </c>
       <c r="C22" s="10"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B23" s="7" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B24" s="7" t="s">
-        <v>116</v>
+        <v>66</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>117</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.45">
@@ -2898,10 +2438,10 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B26" s="8" t="s">
-        <v>118</v>
+        <v>68</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>119</v>
+        <v>69</v>
       </c>
       <c r="D26" s="6">
         <v>2</v>
@@ -2914,7 +2454,7 @@
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B29" s="6" t="s">
-        <v>124</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.45">
@@ -2951,7 +2491,7 @@
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B36" s="6" t="s">
-        <v>125</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.45">
@@ -2965,24 +2505,24 @@
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B38" s="10" t="s">
-        <v>135</v>
+        <v>85</v>
       </c>
       <c r="C38" s="10"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B39" s="7" t="s">
-        <v>132</v>
+        <v>82</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>133</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B40" s="7" t="s">
-        <v>116</v>
+        <v>66</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>117</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.45">
@@ -3025,7 +2565,7 @@
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B47" s="6" t="s">
-        <v>126</v>
+        <v>76</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.45">
@@ -3070,7 +2610,7 @@
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B54" s="6" t="s">
-        <v>127</v>
+        <v>77</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.45">
@@ -3084,24 +2624,24 @@
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B56" s="10" t="s">
-        <v>136</v>
+        <v>86</v>
       </c>
       <c r="C56" s="10"/>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B57" s="7" t="s">
-        <v>132</v>
+        <v>82</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>133</v>
+        <v>83</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B58" s="7" t="s">
-        <v>116</v>
+        <v>66</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>117</v>
+        <v>67</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.45">
@@ -3131,7 +2671,7 @@
         <v>23</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="D61" s="6">
         <v>3</v>
@@ -3144,7 +2684,7 @@
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B65" s="6" t="s">
-        <v>128</v>
+        <v>78</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.45">
@@ -3202,7 +2742,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1419F7E2-9043-468E-84C5-EE71ECF16D61}">
   <dimension ref="A3:J84"/>
   <sheetViews>
@@ -3219,7 +2759,7 @@
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
-        <v>92</v>
+        <v>42</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -3338,7 +2878,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B13" s="3" t="s">
-        <v>93</v>
+        <v>43</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -3433,7 +2973,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B21" s="3" t="s">
-        <v>94</v>
+        <v>44</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -3511,7 +3051,7 @@
     <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" s="3"/>
       <c r="B32" s="3" t="s">
-        <v>95</v>
+        <v>45</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -3568,7 +3108,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B39" s="3" t="s">
-        <v>96</v>
+        <v>46</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -3644,7 +3184,7 @@
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B50" s="3" t="s">
-        <v>97</v>
+        <v>47</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
@@ -3702,7 +3242,7 @@
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B58" s="3" t="s">
-        <v>98</v>
+        <v>48</v>
       </c>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
@@ -3786,7 +3326,7 @@
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B70" s="3" t="s">
-        <v>99</v>
+        <v>49</v>
       </c>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
@@ -3882,11 +3422,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F68DA87-1449-427E-BA16-0FD4624090EF}">
   <dimension ref="C4:G75"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
@@ -3894,7 +3434,7 @@
   <sheetData>
     <row r="4" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C4" s="6" t="s">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -3914,7 +3454,7 @@
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C6" s="6" t="s">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -3982,7 +3522,7 @@
     </row>
     <row r="14" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C14" s="6" t="s">
-        <v>101</v>
+        <v>51</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -4056,7 +3596,7 @@
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C22" s="6" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
@@ -4076,7 +3616,7 @@
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C24" s="6" t="s">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
@@ -4085,7 +3625,7 @@
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C25" s="6" t="s">
-        <v>91</v>
+        <v>41</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
@@ -4155,7 +3695,7 @@
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C33" s="6" t="s">
-        <v>103</v>
+        <v>53</v>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
@@ -4222,7 +3762,7 @@
     </row>
     <row r="40" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C40" s="6" t="s">
-        <v>104</v>
+        <v>54</v>
       </c>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
@@ -4242,7 +3782,7 @@
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C42" s="6" t="s">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
@@ -4321,7 +3861,7 @@
     </row>
     <row r="51" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C51" s="6" t="s">
-        <v>105</v>
+        <v>55</v>
       </c>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
@@ -4395,7 +3935,7 @@
     </row>
     <row r="59" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C59" s="6" t="s">
-        <v>106</v>
+        <v>56</v>
       </c>
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
@@ -4415,7 +3955,7 @@
     </row>
     <row r="61" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C61" s="6" t="s">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="D61" s="6"/>
       <c r="E61" s="6"/>
@@ -4424,7 +3964,7 @@
     </row>
     <row r="62" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C62" s="6" t="s">
-        <v>91</v>
+        <v>41</v>
       </c>
       <c r="D62" s="6"/>
       <c r="E62" s="6"/>
@@ -4505,7 +4045,7 @@
     </row>
     <row r="71" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C71" s="6" t="s">
-        <v>107</v>
+        <v>57</v>
       </c>
       <c r="D71" s="6"/>
       <c r="E71" s="6"/>
@@ -4561,12 +4101,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E62FB8E-0217-4AE2-A967-927A634148DB}">
   <dimension ref="B3:C74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4579,7 +4119,7 @@
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B3" s="6" t="s">
-        <v>137</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.45">
@@ -4597,7 +4137,7 @@
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B6" s="6" t="s">
-        <v>143</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.45">
@@ -4607,7 +4147,7 @@
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B8" s="6" t="s">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="C8" s="6">
         <v>1</v>
@@ -4620,7 +4160,7 @@
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B13" s="6" t="s">
-        <v>151</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.45">
@@ -4657,7 +4197,7 @@
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B21" s="6" t="s">
-        <v>138</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.45">
@@ -4675,7 +4215,7 @@
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B24" s="6" t="s">
-        <v>144</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.45">
@@ -4685,7 +4225,7 @@
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B26" s="5" t="s">
-        <v>145</v>
+        <v>95</v>
       </c>
       <c r="C26" s="6">
         <v>1</v>
@@ -4706,7 +4246,7 @@
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B32" s="6" t="s">
-        <v>152</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.45">
@@ -4743,7 +4283,7 @@
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B39" s="6" t="s">
-        <v>139</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.45">
@@ -4761,7 +4301,7 @@
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B42" s="6" t="s">
-        <v>143</v>
+        <v>93</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.45">
@@ -4771,7 +4311,7 @@
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B44" s="6" t="s">
-        <v>146</v>
+        <v>96</v>
       </c>
       <c r="C44" s="6">
         <v>1</v>
@@ -4779,7 +4319,7 @@
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B45" s="4" t="s">
-        <v>147</v>
+        <v>97</v>
       </c>
       <c r="C45" s="6">
         <v>2</v>
@@ -4792,7 +4332,7 @@
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B50" s="6" t="s">
-        <v>140</v>
+        <v>90</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.45">
@@ -4829,7 +4369,7 @@
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B58" s="6" t="s">
-        <v>141</v>
+        <v>91</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.45">
@@ -4847,7 +4387,7 @@
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B61" s="6" t="s">
-        <v>144</v>
+        <v>94</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.45">
@@ -4857,7 +4397,7 @@
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B63" s="5" t="s">
-        <v>145</v>
+        <v>95</v>
       </c>
       <c r="C63" s="6">
         <v>1</v>
@@ -4865,7 +4405,7 @@
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B64" s="5" t="s">
-        <v>148</v>
+        <v>98</v>
       </c>
       <c r="C64" s="6">
         <v>2</v>
@@ -4873,7 +4413,7 @@
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B65" s="4" t="s">
-        <v>149</v>
+        <v>99</v>
       </c>
       <c r="C65" s="6">
         <v>3</v>
@@ -4886,7 +4426,372 @@
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B70" s="6" t="s">
-        <v>142</v>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B71" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B72" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B73" s="6">
+        <v>12</v>
+      </c>
+      <c r="C73" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B74" s="6">
+        <v>112</v>
+      </c>
+      <c r="C74" s="6">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6D1D285-ADEB-4203-A39D-42362C353566}">
+  <dimension ref="B3:C74"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="9.06640625" style="6" collapsed="1"/>
+    <col min="2" max="2" width="19.33203125" style="6" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.9296875" style="6" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.06640625" style="6" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B3" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B5" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B6" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B7" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B8" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="C9" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B13" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B17" s="6">
+        <v>12</v>
+      </c>
+      <c r="C17" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B21" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B23" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B24" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B25" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B26" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B27" s="6">
+        <v>112</v>
+      </c>
+      <c r="C27" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="C28" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B32" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B33" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B34" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B35" s="6">
+        <v>12</v>
+      </c>
+      <c r="C35" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B36" s="6">
+        <v>112</v>
+      </c>
+      <c r="C36" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B39" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B40" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B41" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B42" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B43" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B44" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C44" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B45" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C45" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="C46" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B50" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B51" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B52" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B53" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C53" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B54" s="5">
+        <v>12</v>
+      </c>
+      <c r="C54" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B58" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B59" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B60" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B61" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B62" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B63" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C63" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B64" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C64" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B65" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C65" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="C66" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B70" s="6" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
EPBDS-9039 Incorrect Cast happens if input value and condition have different types. Fix test for Java 11.
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9039_IndexAndNoIndexDTWithDifferentTypesV1.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9039_IndexAndNoIndexDTWithDifferentTypesV1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C26029-3585-44F9-920B-5FBAF3EE3003}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1611852-4AE9-4DB7-8689-1C92718DA983}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5693" yWindow="2318" windowWidth="21600" windowHeight="11535" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Range" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="113">
   <si>
     <t>C1</t>
   </si>
@@ -102,9 +102,6 @@
     <t>12.1</t>
   </si>
   <si>
-    <t>= new Integer(-100)</t>
-  </si>
-  <si>
     <t>= new Double(-100)</t>
   </si>
   <si>
@@ -240,12 +237,6 @@
     <t>Max</t>
   </si>
   <si>
-    <t>=new Integer(-100)</t>
-  </si>
-  <si>
-    <t>=new Integer(-99)</t>
-  </si>
-  <si>
     <t>= new Double(-99)</t>
   </si>
   <si>
@@ -376,6 +367,12 @@
   </si>
   <si>
     <t>Double[] x</t>
+  </si>
+  <si>
+    <t>= Integer.valueOf(-100)</t>
+  </si>
+  <si>
+    <t>= Integer.valueOf(-99)</t>
   </si>
 </sst>
 </file>
@@ -843,7 +840,7 @@
     </row>
     <row r="9" spans="2:3" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="3">
         <v>2</v>
@@ -937,7 +934,7 @@
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B26" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C26">
         <v>2</v>
@@ -1077,7 +1074,7 @@
     <row r="42" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C42" s="1">
         <v>2</v>
@@ -1254,7 +1251,7 @@
     </row>
     <row r="59" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B59" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C59" s="3">
         <v>2</v>
@@ -1262,7 +1259,7 @@
     </row>
     <row r="60" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B60" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C60" s="1">
         <v>3</v>
@@ -1337,7 +1334,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA0AAF78-1E59-425E-A306-262A8A76F550}">
   <dimension ref="B3:C69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
@@ -1345,7 +1342,7 @@
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B3" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="3"/>
     </row>
@@ -1359,13 +1356,13 @@
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B5" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="3"/>
     </row>
@@ -1385,7 +1382,7 @@
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="3">
         <v>2</v>
@@ -1403,7 +1400,7 @@
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B12" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" s="3"/>
     </row>
@@ -1457,7 +1454,7 @@
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B20" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20" s="3"/>
     </row>
@@ -1471,13 +1468,13 @@
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B22" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C22" s="3"/>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B23" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23" s="3"/>
     </row>
@@ -1497,7 +1494,7 @@
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B26" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C26" s="3">
         <v>2</v>
@@ -1515,7 +1512,7 @@
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B29" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C29" s="3"/>
     </row>
@@ -1557,7 +1554,7 @@
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B36" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C36" s="3"/>
     </row>
@@ -1571,13 +1568,13 @@
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B38" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C38" s="3"/>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B39" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C39" s="3"/>
     </row>
@@ -1597,7 +1594,7 @@
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B42" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C42" s="3">
         <v>2</v>
@@ -1619,7 +1616,7 @@
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B46" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C46" s="3"/>
     </row>
@@ -1669,7 +1666,7 @@
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B53" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C53" s="3"/>
     </row>
@@ -1683,13 +1680,13 @@
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B55" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C55" s="3"/>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B56" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C56" s="3"/>
     </row>
@@ -1709,7 +1706,7 @@
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B59" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C59" s="3">
         <v>2</v>
@@ -1717,7 +1714,7 @@
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B60" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C60" s="3">
         <v>3</v>
@@ -1739,7 +1736,7 @@
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B64" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C64" s="3"/>
     </row>
@@ -1792,8 +1789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EBBA327-A503-4137-A681-2390B6DD3420}">
   <dimension ref="B3:D70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1806,7 +1803,7 @@
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B3" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.45">
@@ -1834,10 +1831,10 @@
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B7" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.45">
@@ -1869,7 +1866,7 @@
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B12" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.45">
@@ -1914,7 +1911,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B20" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.45">
@@ -1942,10 +1939,10 @@
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B24" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.45">
@@ -1961,10 +1958,10 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B26" s="8" t="s">
-        <v>68</v>
+        <v>111</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>69</v>
+        <v>112</v>
       </c>
       <c r="D26" s="6">
         <v>2</v>
@@ -1977,7 +1974,7 @@
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B29" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.45">
@@ -2014,7 +2011,7 @@
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B36" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.45">
@@ -2042,10 +2039,10 @@
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B40" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.45">
@@ -2088,7 +2085,7 @@
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B47" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.45">
@@ -2133,7 +2130,7 @@
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B54" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.45">
@@ -2161,10 +2158,10 @@
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B58" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C58" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="C58" s="7" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.45">
@@ -2191,10 +2188,10 @@
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B61" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D61" s="6">
         <v>3</v>
@@ -2207,7 +2204,7 @@
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B65" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.45">
@@ -2269,8 +2266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAEE3FEA-B42F-4DA8-AFDC-3595C7CB86E9}">
   <dimension ref="B3:D70"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36:D44"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2283,7 +2280,7 @@
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B3" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.45">
@@ -2297,24 +2294,24 @@
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B5" s="10" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C5" s="10"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B6" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B7" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.45">
@@ -2346,7 +2343,7 @@
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B12" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.45">
@@ -2391,7 +2388,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B20" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.45">
@@ -2405,24 +2402,24 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B22" s="10" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C22" s="10"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B23" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B24" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.45">
@@ -2438,10 +2435,10 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B26" s="8" t="s">
-        <v>68</v>
+        <v>111</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>69</v>
+        <v>112</v>
       </c>
       <c r="D26" s="6">
         <v>2</v>
@@ -2454,7 +2451,7 @@
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B29" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.45">
@@ -2491,7 +2488,7 @@
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B36" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.45">
@@ -2505,24 +2502,24 @@
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B38" s="10" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C38" s="10"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B39" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B40" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.45">
@@ -2565,7 +2562,7 @@
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B47" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.45">
@@ -2610,7 +2607,7 @@
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B54" s="6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.45">
@@ -2624,24 +2621,24 @@
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B56" s="10" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C56" s="10"/>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B57" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B58" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C58" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="C58" s="7" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.45">
@@ -2668,10 +2665,10 @@
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B61" s="4" t="s">
-        <v>23</v>
+        <v>111</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>70</v>
+        <v>112</v>
       </c>
       <c r="D61" s="6">
         <v>3</v>
@@ -2684,7 +2681,7 @@
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B65" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.45">
@@ -2746,8 +2743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1419F7E2-9043-468E-84C5-EE71ECF16D61}">
   <dimension ref="A3:J84"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2759,7 +2756,7 @@
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -2878,7 +2875,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B13" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -2973,7 +2970,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B21" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -3051,7 +3048,7 @@
     <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" s="3"/>
       <c r="B32" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -3108,7 +3105,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B39" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -3131,7 +3128,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B42" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -3154,7 +3151,7 @@
     </row>
     <row r="45" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B45" s="4" t="s">
-        <v>22</v>
+        <v>111</v>
       </c>
       <c r="C45" s="3">
         <v>2</v>
@@ -3184,7 +3181,7 @@
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B50" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
@@ -3242,7 +3239,7 @@
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B58" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
@@ -3296,7 +3293,7 @@
     </row>
     <row r="65" spans="2:4" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B65" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C65" s="3">
         <v>3</v>
@@ -3326,7 +3323,7 @@
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B70" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
@@ -3426,15 +3423,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F68DA87-1449-427E-BA16-0FD4624090EF}">
   <dimension ref="C4:G75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="4" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C4" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -3454,7 +3451,7 @@
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C6" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -3463,7 +3460,7 @@
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C7" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -3522,7 +3519,7 @@
     </row>
     <row r="14" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C14" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -3596,7 +3593,7 @@
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C22" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
@@ -3616,7 +3613,7 @@
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C24" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
@@ -3625,7 +3622,7 @@
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C25" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
@@ -3695,7 +3692,7 @@
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C33" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
@@ -3762,7 +3759,7 @@
     </row>
     <row r="40" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C40" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
@@ -3782,7 +3779,7 @@
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C42" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
@@ -3791,7 +3788,7 @@
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C43" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
@@ -3820,7 +3817,7 @@
     </row>
     <row r="46" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C46" s="4" t="s">
-        <v>22</v>
+        <v>111</v>
       </c>
       <c r="D46" s="6">
         <v>2</v>
@@ -3861,7 +3858,7 @@
     </row>
     <row r="51" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C51" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
@@ -3935,7 +3932,7 @@
     </row>
     <row r="59" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C59" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
@@ -3955,7 +3952,7 @@
     </row>
     <row r="61" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C61" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D61" s="6"/>
       <c r="E61" s="6"/>
@@ -3964,7 +3961,7 @@
     </row>
     <row r="62" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C62" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D62" s="6"/>
       <c r="E62" s="6"/>
@@ -4004,7 +4001,7 @@
     </row>
     <row r="66" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C66" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D66" s="6">
         <v>3</v>
@@ -4045,7 +4042,7 @@
     </row>
     <row r="71" spans="3:7" x14ac:dyDescent="0.45">
       <c r="C71" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D71" s="6"/>
       <c r="E71" s="6"/>
@@ -4105,8 +4102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E62FB8E-0217-4AE2-A967-927A634148DB}">
   <dimension ref="B3:C74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4119,7 +4116,7 @@
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B3" s="6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.45">
@@ -4137,7 +4134,7 @@
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B6" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.45">
@@ -4147,7 +4144,7 @@
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B8" s="6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C8" s="6">
         <v>1</v>
@@ -4160,7 +4157,7 @@
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B13" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.45">
@@ -4197,7 +4194,7 @@
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B21" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.45">
@@ -4215,7 +4212,7 @@
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B24" s="6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.45">
@@ -4225,7 +4222,7 @@
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B26" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C26" s="6">
         <v>1</v>
@@ -4246,7 +4243,7 @@
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B32" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.45">
@@ -4283,7 +4280,7 @@
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B39" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.45">
@@ -4301,7 +4298,7 @@
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B42" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.45">
@@ -4311,7 +4308,7 @@
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B44" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C44" s="6">
         <v>1</v>
@@ -4319,7 +4316,7 @@
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B45" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C45" s="6">
         <v>2</v>
@@ -4332,7 +4329,7 @@
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B50" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.45">
@@ -4369,7 +4366,7 @@
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B58" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.45">
@@ -4387,7 +4384,7 @@
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B61" s="6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.45">
@@ -4397,7 +4394,7 @@
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B63" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C63" s="6">
         <v>1</v>
@@ -4405,7 +4402,7 @@
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B64" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C64" s="6">
         <v>2</v>
@@ -4413,7 +4410,7 @@
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B65" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C65" s="6">
         <v>3</v>
@@ -4426,7 +4423,7 @@
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B70" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.45">
@@ -4470,8 +4467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6D1D285-ADEB-4203-A39D-42362C353566}">
   <dimension ref="B3:C74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4484,7 +4481,7 @@
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B3" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.45">
@@ -4497,12 +4494,12 @@
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B5" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B6" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.45">
@@ -4512,7 +4509,7 @@
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B8" s="6" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C8" s="6">
         <v>1</v>
@@ -4525,7 +4522,7 @@
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B13" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.45">
@@ -4562,7 +4559,7 @@
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B21" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.45">
@@ -4575,12 +4572,12 @@
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B23" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B24" s="6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.45">
@@ -4590,7 +4587,7 @@
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B26" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C26" s="6">
         <v>1</v>
@@ -4611,7 +4608,7 @@
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B32" s="6" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.45">
@@ -4648,7 +4645,7 @@
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B39" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.45">
@@ -4661,12 +4658,12 @@
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B41" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B42" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.45">
@@ -4676,7 +4673,7 @@
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B44" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C44" s="6">
         <v>1</v>
@@ -4684,7 +4681,7 @@
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B45" s="4" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="C45" s="6">
         <v>2</v>
@@ -4697,7 +4694,7 @@
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B50" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.45">
@@ -4734,7 +4731,7 @@
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B58" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.45">
@@ -4747,12 +4744,12 @@
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B60" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B61" s="6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.45">
@@ -4762,7 +4759,7 @@
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B63" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C63" s="6">
         <v>1</v>
@@ -4770,7 +4767,7 @@
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B64" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C64" s="6">
         <v>2</v>
@@ -4778,7 +4775,7 @@
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B65" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C65" s="6">
         <v>3</v>
@@ -4791,7 +4788,7 @@
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B70" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
EPBDS-9065 Incorrect Cast happens if input value and condition have different types. Fix and tests.
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9039_IndexAndNoIndexDTWithDifferentTypesV1.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9039_IndexAndNoIndexDTWithDifferentTypesV1.xlsx
@@ -3,24 +3,25 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkama\.openl\user-workspace\DEFAULT\EPBDS-9039_IndexAndNoIndexDTWithDifferentTypesV1_NEW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E7BBED-CFAD-4C5F-B0B4-97BC61018E54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F470902A-D062-4B8E-82B1-A5DD0BB61377}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1688" yWindow="2970" windowWidth="21600" windowHeight="11535" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Range" sheetId="2" r:id="rId1"/>
-    <sheet name="Range_DependentParams" sheetId="4" r:id="rId2"/>
+    <sheet name="Range_Expression" sheetId="4" r:id="rId2"/>
     <sheet name="Range_2_Columns" sheetId="7" r:id="rId3"/>
     <sheet name="Range_2_Column_Expression" sheetId="8" r:id="rId4"/>
     <sheet name="Equals" sheetId="3" r:id="rId5"/>
     <sheet name="Equals_Expression" sheetId="6" r:id="rId6"/>
     <sheet name="Contains" sheetId="9" r:id="rId7"/>
     <sheet name="Contains_Expression" sheetId="10" r:id="rId8"/>
+    <sheet name="Relation" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="125">
   <si>
     <t>C1</t>
   </si>
@@ -373,16 +374,53 @@
   </si>
   <si>
     <t>= Double.valueOf(-99)</t>
+  </si>
+  <si>
+    <t>param &lt; x</t>
+  </si>
+  <si>
+    <t>= Integer.valueOf(12)</t>
+  </si>
+  <si>
+    <t>Rules Integer indexInt_Relation_ParamDouble(Double param)</t>
+  </si>
+  <si>
+    <t>Test indexInt_Relation_ParamDouble indexInt_Relation_ParamDoubleTest</t>
+  </si>
+  <si>
+    <t>Rules Integer noIndexInt_Relation_ParamDouble(Double param)</t>
+  </si>
+  <si>
+    <t>Test noIndexInt_Relation_ParamDouble noIndexInt_Relation_ParamDoubleTest</t>
+  </si>
+  <si>
+    <t>Rules Integer indexDouble_Relation_ParamInteger(Integer param)</t>
+  </si>
+  <si>
+    <t>Test  indexDouble_Relation_ParamInteger indexDouble_Relation_ParamIntegerTest</t>
+  </si>
+  <si>
+    <t>Rules Integer noIndexDouble_Relation_ParamInteger(Integer param)</t>
+  </si>
+  <si>
+    <t>Test  noIndexDouble_Relation_ParamInteger noIndexDouble_Relation_ParamIntegerTest</t>
+  </si>
+  <si>
+    <t>= Double.valueOf(12.1)</t>
+  </si>
+  <si>
+    <t>0.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="1" rgb="000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -406,9 +444,9 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -420,6 +458,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -792,14 +831,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:J69"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="27.796875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.86328125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="27.796875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.86328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.45">
@@ -1334,7 +1373,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA0AAF78-1E59-425E-A306-262A8A76F550}">
   <dimension ref="B3:C69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
@@ -1795,10 +1834,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.06640625" style="6" collapsed="1"/>
-    <col min="2" max="2" width="27.796875" style="6" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.86328125" style="6" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.06640625" style="6" collapsed="1"/>
+    <col min="1" max="1" style="6" width="9.06640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="6" width="27.796875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="6" width="27.86328125" collapsed="true"/>
+    <col min="4" max="16384" style="6" width="9.06640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.45">
@@ -1807,19 +1846,19 @@
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B4" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="10"/>
+      <c r="B4" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="11"/>
       <c r="D4" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B5" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="10"/>
+      <c r="B5" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="11"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B6" s="7" t="s">
@@ -1915,19 +1954,19 @@
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B21" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="10"/>
+      <c r="B21" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="11"/>
       <c r="D21" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B22" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="10"/>
+      <c r="B22" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="11"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B23" s="7" t="s">
@@ -2015,19 +2054,19 @@
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B37" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C37" s="10"/>
+      <c r="B37" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="11"/>
       <c r="D37" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B38" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C38" s="10"/>
+      <c r="B38" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="11"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B39" s="7" t="s">
@@ -2134,19 +2173,19 @@
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B55" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C55" s="10"/>
+      <c r="B55" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C55" s="11"/>
       <c r="D55" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B56" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C56" s="10"/>
+      <c r="B56" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C56" s="11"/>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B57" s="7" t="s">
@@ -2272,10 +2311,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.06640625" style="6" collapsed="1"/>
-    <col min="2" max="2" width="27.796875" style="6" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.86328125" style="6" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.06640625" style="6" collapsed="1"/>
+    <col min="1" max="1" style="6" width="9.06640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="6" width="27.796875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="6" width="27.86328125" collapsed="true"/>
+    <col min="4" max="16384" style="6" width="9.06640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.45">
@@ -2284,19 +2323,19 @@
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B4" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="10"/>
+      <c r="B4" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="11"/>
       <c r="D4" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="10"/>
+      <c r="C5" s="11"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B6" s="7" t="s">
@@ -2392,19 +2431,19 @@
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B21" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="10"/>
+      <c r="B21" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="11"/>
       <c r="D21" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="C22" s="10"/>
+      <c r="C22" s="11"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B23" s="7" t="s">
@@ -2492,19 +2531,19 @@
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B37" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C37" s="10"/>
+      <c r="B37" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="11"/>
       <c r="D37" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C38" s="10"/>
+      <c r="C38" s="11"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B39" s="7" t="s">
@@ -2611,19 +2650,19 @@
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B55" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C55" s="10"/>
+      <c r="B55" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C55" s="11"/>
       <c r="D55" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B56" s="10" t="s">
+      <c r="B56" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="C56" s="10"/>
+      <c r="C56" s="11"/>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B57" s="7" t="s">
@@ -2743,14 +2782,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1419F7E2-9043-468E-84C5-EE71ECF16D61}">
   <dimension ref="A3:J84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="19.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.9296875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="19.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.9296875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
@@ -4108,10 +4147,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.06640625" style="6" collapsed="1"/>
-    <col min="2" max="2" width="19.33203125" style="6" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.9296875" style="6" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.06640625" style="6" collapsed="1"/>
+    <col min="1" max="1" style="6" width="9.06640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="6" width="19.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="6" width="14.9296875" collapsed="true"/>
+    <col min="4" max="16384" style="6" width="9.06640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.45">
@@ -4473,10 +4512,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.06640625" style="6" collapsed="1"/>
-    <col min="2" max="2" width="19.33203125" style="6" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.9296875" style="6" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.06640625" style="6" collapsed="1"/>
+    <col min="1" max="1" style="6" width="9.06640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="6" width="19.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="6" width="14.9296875" collapsed="true"/>
+    <col min="4" max="16384" style="6" width="9.06640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.45">
@@ -4826,4 +4865,410 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BB95D71-539A-4D65-B2D7-37F74449D91F}">
+  <dimension ref="B4:C69"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" customWidth="true" width="31.59765625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="69.265625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B4" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B6" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B9" s="6">
+        <v>12</v>
+      </c>
+      <c r="C9" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B10" s="6"/>
+      <c r="C10" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B12" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B15" s="10">
+        <v>11.99</v>
+      </c>
+      <c r="C15" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B16" s="6">
+        <v>12.1</v>
+      </c>
+      <c r="C16" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B20" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C20" s="6"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B22" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C22" s="6"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B23" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="6"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B24" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="6"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B25" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C25" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B26" s="6"/>
+      <c r="C26" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B29" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C29" s="6"/>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B30" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B31" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B32" s="10">
+        <v>11.99</v>
+      </c>
+      <c r="C32" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B33" s="6">
+        <v>12.1</v>
+      </c>
+      <c r="C33" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B36" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C36" s="6"/>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B37" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B38" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C38" s="6"/>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B39" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" s="6"/>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B40" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" s="6"/>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B41" s="6">
+        <v>12.1</v>
+      </c>
+      <c r="C41" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B42" s="6"/>
+      <c r="C42" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B46" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C46" s="6"/>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B47" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B48" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B49" s="6">
+        <v>12</v>
+      </c>
+      <c r="C49" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B50" s="6">
+        <v>13</v>
+      </c>
+      <c r="C50" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B53" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C53" s="6"/>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B54" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B55" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C55" s="6"/>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B56" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C56" s="6"/>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B57" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C57" s="6"/>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B58" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C58" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B59" s="6"/>
+      <c r="C59" t="n" s="6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.45"/>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.45"/>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B62" s="6"/>
+      <c r="C62" s="6"/>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B63" s="6"/>
+      <c r="C63" s="6"/>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B64" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C64" s="6"/>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B65" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B66" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B67" t="n" s="6">
+        <v>12.0</v>
+      </c>
+      <c r="C67" t="n" s="6">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B68" s="6" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="C68" s="6" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.45"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>